<commit_message>
+ upload SRS samples/ORMS_SRS_v1.2_EN.docx + done SE18_SRS_v2.0
</commit_message>
<xml_diff>
--- a/2. SRS/v1.0/SRS_Review_CheckList(SE18).xlsx
+++ b/2. SRS/v1.0/SRS_Review_CheckList(SE18).xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\001_IT BOOK\Nam 4\2. Ky II\Do an CNPM\[DO AN] Nhom Chanh, Binh, Dung, Cung\trunk\2. SRS\v1.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="19065" windowHeight="11760"/>
   </bookViews>
@@ -634,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -770,6 +775,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,7 +848,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -866,7 +883,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1077,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E23" sqref="A23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1347,15 +1364,15 @@
       <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6" ht="120">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="36" t="s">
+      <c r="B23" s="47"/>
+      <c r="C23" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="48" t="s">
         <v>53</v>
       </c>
       <c r="F23" s="40"/>
@@ -1453,29 +1470,29 @@
       <c r="F31" s="40"/>
     </row>
     <row r="32" spans="1:6" ht="60">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="36" t="s">
+      <c r="B32" s="47"/>
+      <c r="C32" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="47"/>
+      <c r="E32" s="48" t="s">
         <v>56</v>
       </c>
       <c r="F32" s="40"/>
     </row>
     <row r="33" spans="1:6" ht="36">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="36" t="s">
+      <c r="B33" s="47"/>
+      <c r="C33" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="47"/>
+      <c r="E33" s="48" t="s">
         <v>60</v>
       </c>
       <c r="F33" s="40" t="s">

</xml_diff>